<commit_message>
making adjustments to scripts
</commit_message>
<xml_diff>
--- a/Документация/Расчет нагрузки профиля итог на 20 минут 6 операций.xlsx
+++ b/Документация/Расчет нагрузки профиля итог на 20 минут 6 операций.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6885" windowHeight="6330" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6885" windowHeight="6330"/>
   </bookViews>
   <sheets>
     <sheet name="Расчетная таблица" sheetId="1" r:id="rId1"/>
@@ -1395,44 +1395,44 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="36" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="36" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="36" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2948,8 +2948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2969,22 +2969,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="104" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="104"/>
     </row>
     <row r="3" spans="1:22" s="6" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="96" t="s">
@@ -3404,15 +3404,15 @@
       <c r="N12" s="77"/>
     </row>
     <row r="13" spans="1:22" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="104" t="s">
+      <c r="A13" s="105" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="104"/>
-      <c r="C13" s="104"/>
-      <c r="D13" s="104"/>
-      <c r="E13" s="104"/>
-      <c r="F13" s="104"/>
-      <c r="G13" s="104"/>
+      <c r="B13" s="105"/>
+      <c r="C13" s="105"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="105"/>
+      <c r="F13" s="105"/>
+      <c r="G13" s="105"/>
       <c r="H13" s="74"/>
       <c r="I13" s="74"/>
       <c r="J13" s="75"/>
@@ -3431,19 +3431,19 @@
       <c r="C15" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="99" t="s">
+      <c r="D15" s="106" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="100"/>
-      <c r="F15" s="99" t="s">
+      <c r="E15" s="107"/>
+      <c r="F15" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="100"/>
+      <c r="G15" s="107"/>
       <c r="H15" s="19"/>
-      <c r="I15" s="105" t="s">
+      <c r="I15" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="106"/>
+      <c r="J15" s="100"/>
       <c r="K15" s="98" t="s">
         <v>73</v>
       </c>
@@ -3477,8 +3477,8 @@
       <c r="G16" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="I16" s="105"/>
-      <c r="J16" s="106"/>
+      <c r="I16" s="99"/>
+      <c r="J16" s="100"/>
       <c r="K16" s="98"/>
       <c r="L16" s="97"/>
       <c r="M16" s="38"/>
@@ -3517,10 +3517,10 @@
         <f t="shared" ref="G17:G20" ca="1" si="8">1-D17/F17</f>
         <v>-4.6620046620047262E-3</v>
       </c>
-      <c r="I17" s="107" t="s">
+      <c r="I17" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="J17" s="107"/>
+      <c r="J17" s="95"/>
       <c r="K17" s="44">
         <v>0.74099999999999999</v>
       </c>
@@ -3563,10 +3563,10 @@
         <f t="shared" ca="1" si="8"/>
         <v>1.631701631701632E-2</v>
       </c>
-      <c r="I18" s="107" t="s">
+      <c r="I18" s="95" t="s">
         <v>41</v>
       </c>
-      <c r="J18" s="107"/>
+      <c r="J18" s="95"/>
       <c r="K18" s="44">
         <v>0.74099999999999999</v>
       </c>
@@ -3609,10 +3609,10 @@
         <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
-      <c r="I19" s="107" t="s">
+      <c r="I19" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="J19" s="107"/>
+      <c r="J19" s="95"/>
       <c r="K19" s="44">
         <v>0.74099999999999999</v>
       </c>
@@ -3655,10 +3655,10 @@
         <f t="shared" ca="1" si="8"/>
         <v>2.422145328719727E-2</v>
       </c>
-      <c r="I20" s="107" t="s">
+      <c r="I20" s="95" t="s">
         <v>43</v>
       </c>
-      <c r="J20" s="107"/>
+      <c r="J20" s="95"/>
       <c r="K20" s="44">
         <v>0.74099999999999999</v>
       </c>
@@ -3702,10 +3702,10 @@
         <v>7.905138339920903E-3</v>
       </c>
       <c r="H21" s="41"/>
-      <c r="I21" s="107" t="s">
+      <c r="I21" s="95" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="107"/>
+      <c r="J21" s="95"/>
       <c r="K21" s="44">
         <v>0.74099999999999999</v>
       </c>
@@ -3748,10 +3748,10 @@
         <f t="shared" ref="G22:G26" ca="1" si="9">1-D22/F22</f>
         <v>2.777777777777779E-2</v>
       </c>
-      <c r="I22" s="107" t="s">
+      <c r="I22" s="95" t="s">
         <v>62</v>
       </c>
-      <c r="J22" s="107"/>
+      <c r="J22" s="95"/>
       <c r="K22" s="45">
         <v>0.74099999999999999</v>
       </c>
@@ -3928,12 +3928,12 @@
       <c r="O28"/>
     </row>
     <row r="29" spans="1:22" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="95" t="s">
+      <c r="A29" s="104" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="95"/>
-      <c r="C29" s="95"/>
-      <c r="D29" s="95"/>
+      <c r="B29" s="104"/>
+      <c r="C29" s="104"/>
+      <c r="D29" s="104"/>
       <c r="H29" s="25"/>
       <c r="I29" s="25"/>
       <c r="J29" s="39"/>
@@ -4150,17 +4150,10 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="I15:J16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="A29:D29"/>
@@ -4177,10 +4170,17 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="J3:J4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="I15:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="B15:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="63" orientation="landscape" r:id="rId1"/>
@@ -5538,8 +5538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5557,17 +5557,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="104" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
     </row>
     <row r="3" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="113" t="s">

</xml_diff>